<commit_message>
rahade excel difficulty mode final
</commit_message>
<xml_diff>
--- a/rahad.xlsx
+++ b/rahad.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
   <si>
     <t>type_1</t>
   </si>
@@ -1263,12 +1263,21 @@
   <si>
     <t>money per house per sec</t>
   </si>
+  <si>
+    <t>easy</t>
+  </si>
+  <si>
+    <t>self.right_button_prices</t>
+  </si>
+  <si>
+    <t>insane</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1344,6 +1353,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1353,7 +1369,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1441,16 +1457,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1472,6 +1524,25 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1752,24 +1823,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:L28"/>
+  <dimension ref="A3:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29" style="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="114.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G3" s="19"/>
+    </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L4" s="1" t="s">
         <v>8</v>
@@ -1786,311 +1862,624 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="17" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="9"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="29"/>
       <c r="L7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E8" s="15"/>
-      <c r="F8" s="11" t="s">
+      <c r="E8" s="14"/>
+      <c r="F8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="11" t="s">
         <v>15</v>
+      </c>
+      <c r="J8" s="26" t="s">
+        <v>17</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>10</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>1</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="6">
         <v>0</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <f>F9*G9</f>
         <v>10</v>
       </c>
+      <c r="J9" s="27">
+        <v>1500</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>30</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <v>3</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="6">
         <v>40</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="5">
         <f>F10*G10</f>
         <v>90</v>
       </c>
+      <c r="J10" s="27">
+        <v>1800</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>80</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <v>8</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="6">
         <v>160</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="5">
         <f>F11*G11</f>
         <v>640</v>
       </c>
+      <c r="J11" s="27">
+        <v>8000</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>180</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="6">
         <v>18</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="6">
         <v>540</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="5">
         <f>F12*G12</f>
         <v>3240</v>
       </c>
+      <c r="J12" s="27">
+        <v>972000</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="12">
         <v>450</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="12">
         <v>45</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="12">
         <v>1200</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="7">
         <f>F13*G13</f>
         <v>20250</v>
       </c>
+      <c r="J13" s="28">
+        <v>5062500</v>
+      </c>
     </row>
     <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="5"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="19"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="25"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E16" s="15"/>
-      <c r="F16" s="11" t="s">
+      <c r="E16" s="14"/>
+      <c r="F16" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="11" t="s">
         <v>15</v>
       </c>
+      <c r="J16" s="26" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="17" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <v>10</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="6">
         <v>1</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="6">
         <v>0</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="5">
         <f>F17*G17</f>
         <v>10</v>
       </c>
+      <c r="J17" s="27">
+        <v>1500</v>
+      </c>
     </row>
     <row r="18" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="6">
         <v>45</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="6">
         <v>2</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="6">
         <v>60</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="5">
         <f>F18*G18</f>
         <v>90</v>
       </c>
+      <c r="J18" s="27">
+        <v>1800</v>
+      </c>
     </row>
     <row r="19" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="6">
         <v>128</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="6">
         <v>5</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="6">
         <v>256</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="5">
         <f>F19*G19</f>
         <v>640</v>
       </c>
+      <c r="J19" s="27">
+        <v>8000</v>
+      </c>
     </row>
     <row r="20" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="6">
         <v>360</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="6">
         <v>9</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="6">
         <v>1080</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I20" s="5">
         <f>F20*G20</f>
         <v>3240</v>
       </c>
+      <c r="J20" s="27">
+        <v>972000</v>
+      </c>
     </row>
     <row r="21" spans="5:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="12">
         <v>675</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="12">
         <v>30</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="12">
         <v>1800</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I21" s="7">
         <f>F21*G21</f>
         <v>20250</v>
       </c>
-      <c r="J21" s="4"/>
-    </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
+      <c r="J21" s="28">
+        <v>5062500</v>
+      </c>
+    </row>
+    <row r="22" spans="5:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="23"/>
     </row>
     <row r="23" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
+      <c r="E23" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="30"/>
     </row>
     <row r="24" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" s="31" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="25" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E25" s="10"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
+      <c r="E25" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" s="6">
+        <v>20</v>
+      </c>
+      <c r="G25" s="6">
+        <v>2</v>
+      </c>
+      <c r="H25" s="6">
+        <v>0</v>
+      </c>
+      <c r="I25" s="5">
+        <f>F25*G25</f>
+        <v>40</v>
+      </c>
+      <c r="J25" s="32">
+        <v>750</v>
+      </c>
     </row>
     <row r="26" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E26" s="10"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
+      <c r="E26" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="6">
+        <v>90</v>
+      </c>
+      <c r="G26" s="6">
+        <v>4</v>
+      </c>
+      <c r="H26" s="6">
+        <v>60</v>
+      </c>
+      <c r="I26" s="5">
+        <f>F26*G26</f>
+        <v>360</v>
+      </c>
+      <c r="J26" s="32">
+        <v>900</v>
+      </c>
     </row>
     <row r="27" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E27" s="11"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
+      <c r="E27" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" s="6">
+        <v>256</v>
+      </c>
+      <c r="G27" s="6">
+        <v>10</v>
+      </c>
+      <c r="H27" s="6">
+        <v>256</v>
+      </c>
+      <c r="I27" s="5">
+        <f>F27*G27</f>
+        <v>2560</v>
+      </c>
+      <c r="J27" s="32">
+        <v>4000</v>
+      </c>
     </row>
     <row r="28" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E28" s="10"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
+      <c r="E28" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" s="6">
+        <v>720</v>
+      </c>
+      <c r="G28" s="6">
+        <v>18</v>
+      </c>
+      <c r="H28" s="6">
+        <v>1080</v>
+      </c>
+      <c r="I28" s="5">
+        <f>F28*G28</f>
+        <v>12960</v>
+      </c>
+      <c r="J28" s="32">
+        <v>486000</v>
+      </c>
+    </row>
+    <row r="29" spans="5:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="12">
+        <v>1350</v>
+      </c>
+      <c r="G29" s="12">
+        <v>60</v>
+      </c>
+      <c r="H29" s="12">
+        <v>1800</v>
+      </c>
+      <c r="I29" s="7">
+        <f>F29*G29</f>
+        <v>81000</v>
+      </c>
+      <c r="J29" s="33">
+        <v>2531250</v>
+      </c>
+    </row>
+    <row r="30" spans="5:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E31" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="30"/>
+    </row>
+    <row r="32" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E32" s="14"/>
+      <c r="F32" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J32" s="31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E33" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" s="6">
+        <v>5</v>
+      </c>
+      <c r="G33" s="6">
+        <v>1</v>
+      </c>
+      <c r="H33" s="6">
+        <v>0</v>
+      </c>
+      <c r="I33" s="5">
+        <f>F33*G33</f>
+        <v>5</v>
+      </c>
+      <c r="J33" s="34">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E34" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" s="6">
+        <v>22</v>
+      </c>
+      <c r="G34" s="6">
+        <v>2</v>
+      </c>
+      <c r="H34" s="6">
+        <v>20</v>
+      </c>
+      <c r="I34" s="5">
+        <f>F34*G34</f>
+        <v>44</v>
+      </c>
+      <c r="J34" s="34">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E35" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" s="6">
+        <v>64</v>
+      </c>
+      <c r="G35" s="6">
+        <v>3</v>
+      </c>
+      <c r="H35" s="6">
+        <v>70</v>
+      </c>
+      <c r="I35" s="5">
+        <f>F35*G35</f>
+        <v>192</v>
+      </c>
+      <c r="J35" s="34">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="36" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E36" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F36" s="6">
+        <v>180</v>
+      </c>
+      <c r="G36" s="6">
+        <v>5</v>
+      </c>
+      <c r="H36" s="6">
+        <v>300</v>
+      </c>
+      <c r="I36" s="5">
+        <f>F36*G36</f>
+        <v>900</v>
+      </c>
+      <c r="J36" s="34">
+        <v>1944000</v>
+      </c>
+    </row>
+    <row r="37" spans="5:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E37" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" s="12">
+        <v>330</v>
+      </c>
+      <c r="G37" s="12">
+        <v>15</v>
+      </c>
+      <c r="H37" s="12">
+        <v>460</v>
+      </c>
+      <c r="I37" s="7">
+        <f>F37*G37</f>
+        <v>4950</v>
+      </c>
+      <c r="J37" s="35">
+        <v>10125000</v>
+      </c>
+    </row>
+    <row r="39" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="24"/>
+    </row>
+    <row r="40" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E40" s="6"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="20"/>
+    </row>
+    <row r="41" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="22"/>
+    </row>
+    <row r="42" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="22"/>
+    </row>
+    <row r="43" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="22"/>
+    </row>
+    <row r="44" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="22"/>
+    </row>
+    <row r="45" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="E7:I7"/>
     <mergeCell ref="E15:I15"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E31:I31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>